<commit_message>
Update Experimet-2 Validation Accuracy Table.xlsx
</commit_message>
<xml_diff>
--- a/Experimet-2 Validation Accuracy Table.xlsx
+++ b/Experimet-2 Validation Accuracy Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgurlek\Desktop\loops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgurlek\Box\Okul\Deep Learning\Music-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8D9FA6-974A-40AB-914D-DD72C8A05206}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A32150-02F5-42C1-A89E-6A6C76A0A84B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1335" windowWidth="13290" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="val" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +377,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -559,7 +566,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -703,6 +710,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -748,7 +786,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -756,17 +794,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1130,7 +1183,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K12" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,12 +1495,12 @@
       <c r="E12">
         <v>0.150208333</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1465,23 +1518,23 @@
       <c r="E13">
         <v>0.171125001</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5" t="s">
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="4">
-        <v>8</v>
-      </c>
-      <c r="O13" s="4">
-        <v>16</v>
-      </c>
-      <c r="P13" s="4">
-        <v>32</v>
-      </c>
-      <c r="Q13" s="4">
+      <c r="N13" s="3">
+        <v>8</v>
+      </c>
+      <c r="O13" s="3">
+        <v>16</v>
+      </c>
+      <c r="P13" s="3">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="3">
         <v>64</v>
       </c>
     </row>
@@ -1501,13 +1554,13 @@
       <c r="E14">
         <v>0.15691666600000001</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="11">
         <v>8</v>
       </c>
       <c r="L14" s="2">
         <v>8</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="7">
         <v>8</v>
       </c>
       <c r="N14" s="1">
@@ -1551,11 +1604,11 @@
       <c r="E15">
         <v>0.14804167200000001</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="2">
         <v>8</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="8">
         <v>16</v>
       </c>
       <c r="N15" s="1">
@@ -1599,11 +1652,11 @@
       <c r="E16">
         <v>0.15541666400000001</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="2">
         <v>8</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="8">
         <v>32</v>
       </c>
       <c r="N16" s="1">
@@ -1647,11 +1700,11 @@
       <c r="E17">
         <v>0.17358333200000001</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="5">
-        <v>8</v>
-      </c>
-      <c r="M17" s="5">
+      <c r="K17" s="13"/>
+      <c r="L17" s="4">
+        <v>8</v>
+      </c>
+      <c r="M17" s="9">
         <v>64</v>
       </c>
       <c r="N17" s="5" t="s">
@@ -1695,13 +1748,13 @@
       <c r="E18">
         <v>0.17404166800000001</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="11">
         <v>16</v>
       </c>
       <c r="L18" s="2">
         <v>16</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="8">
         <v>8</v>
       </c>
       <c r="N18" s="1">
@@ -1745,11 +1798,11 @@
       <c r="E19">
         <v>0.17600000199999999</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="2">
         <v>16</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="8">
         <v>16</v>
       </c>
       <c r="N19" s="1">
@@ -1793,23 +1846,23 @@
       <c r="E20">
         <v>0.19620833100000001</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="2">
         <v>16</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="8">
         <v>32</v>
       </c>
       <c r="N20" s="1">
         <v>0.12189999999999999</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="O20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="P20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="Q20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S20" t="s">
@@ -1841,11 +1894,11 @@
       <c r="E21">
         <v>0.167375001</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="5">
-        <v>16</v>
-      </c>
-      <c r="M21" s="5">
+      <c r="K21" s="13"/>
+      <c r="L21" s="4">
+        <v>16</v>
+      </c>
+      <c r="M21" s="9">
         <v>64</v>
       </c>
       <c r="N21" s="5" t="s">
@@ -1889,13 +1942,13 @@
       <c r="E22">
         <v>0.16895832999999999</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="11">
         <v>32</v>
       </c>
       <c r="L22" s="2">
         <v>32</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="8">
         <v>8</v>
       </c>
       <c r="N22" s="1">
@@ -1939,11 +1992,11 @@
       <c r="E23">
         <v>0.167124999</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="2">
         <v>32</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="8">
         <v>16</v>
       </c>
       <c r="N23" s="1">
@@ -1987,23 +2040,23 @@
       <c r="E24">
         <v>0.16612500299999999</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="2">
         <v>32</v>
       </c>
-      <c r="M24" s="2">
-        <v>32</v>
-      </c>
-      <c r="N24" s="2" t="s">
+      <c r="M24" s="8">
+        <v>32</v>
+      </c>
+      <c r="N24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P24" s="1">
         <v>0.1087</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S24" t="s">
@@ -2035,11 +2088,11 @@
       <c r="E25">
         <v>0.16195833400000001</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="5">
-        <v>32</v>
-      </c>
-      <c r="M25" s="5">
+      <c r="K25" s="13"/>
+      <c r="L25" s="4">
+        <v>32</v>
+      </c>
+      <c r="M25" s="9">
         <v>64</v>
       </c>
       <c r="N25" s="5" t="s">
@@ -2083,13 +2136,13 @@
       <c r="E26">
         <v>0.177458334</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="11">
         <v>64</v>
       </c>
       <c r="L26" s="2">
         <v>64</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="8">
         <v>8</v>
       </c>
       <c r="N26" s="1">
@@ -2133,11 +2186,11 @@
       <c r="E27">
         <v>0.17854166899999999</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="2">
         <v>64</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="8">
         <v>16</v>
       </c>
       <c r="N27" s="1">
@@ -2181,23 +2234,23 @@
       <c r="E28">
         <v>0.108749999</v>
       </c>
-      <c r="K28" s="6"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="2">
         <v>64</v>
       </c>
-      <c r="M28" s="2">
-        <v>32</v>
-      </c>
-      <c r="N28" s="2" t="s">
+      <c r="M28" s="8">
+        <v>32</v>
+      </c>
+      <c r="N28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="O28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="P28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="Q28" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S28" t="s">
@@ -2229,23 +2282,23 @@
       <c r="E29">
         <v>0.19166666600000001</v>
       </c>
-      <c r="K29" s="6"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="2">
         <v>64</v>
       </c>
-      <c r="M29" s="2">
-        <v>64</v>
-      </c>
-      <c r="N29" s="2" t="s">
+      <c r="M29" s="8">
+        <v>64</v>
+      </c>
+      <c r="N29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="O29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="P29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="Q29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S29" t="s">

</xml_diff>